<commit_message>
Excel-Fomatfehler korrigiert -> manuscripts muss neu erstellt werden
</commit_message>
<xml_diff>
--- a/Parzival_Daten_für_manuscripts.yml.xlsx
+++ b/Parzival_Daten_für_manuscripts.yml.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\student\Documents\_STUDIUM\7_HS17_V_Digital_Humanities\_Julia\Dateien_von_Julia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\student\Documents\_STUDIUM\7_HS17_V_Digital_Humanities\_Julia\porjekt_ordner_source\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1090,8 +1090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1137,8 +1137,8 @@
         <v>9.3768309999999992</v>
       </c>
       <c r="F3" t="str">
-        <f>"  -  ["&amp;""""&amp;A3&amp;""""&amp;","&amp;""""&amp;"https://heinztschan.github.io/parzival/show_library.html?"&amp;"lat="&amp;D3&amp;"&amp;lng="&amp;E3&amp;"&amp;lib="&amp;B3&amp;"&amp;url="&amp;C3&amp;""""&amp;"]"</f>
-        <v xml:space="preserve">  -  ["Hs. D","https://heinztschan.github.io/parzival/show_library.html?lat=47.42318&amp;lng=9.376831&amp;lib=St. Gallen&amp;url=www.parzival.unibe.ch/hsverz.html#1"]</v>
+        <f>"  -  ["&amp;""""&amp;A3&amp;""""&amp;","&amp;""""&amp;"https://heinztschan.github.io/parzival/show_library.html?"&amp;"lat="&amp;D3&amp;"&amp;lng="&amp;E3&amp;"&amp;lib="&amp;B3&amp;"&amp;url=http://"&amp;C3&amp;""""&amp;"]"</f>
+        <v xml:space="preserve">  -  ["Hs. D","https://heinztschan.github.io/parzival/show_library.html?lat=47.42318&amp;lng=9.376831&amp;lib=St. Gallen&amp;url=http://www.parzival.unibe.ch/hsverz.html#1"]</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1158,8 +1158,8 @@
         <v>16.366904000000002</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F67" si="0">"  -  ["&amp;""""&amp;A4&amp;""""&amp;","&amp;""""&amp;"https://heinztschan.github.io/parzival/show_library.html?"&amp;"lat="&amp;D4&amp;"&amp;lng="&amp;E4&amp;"&amp;lib="&amp;B4&amp;"&amp;url="&amp;C4&amp;""""&amp;"]"</f>
-        <v xml:space="preserve">  -  ["Hs. m","https://heinztschan.github.io/parzival/show_library.html?lat=48.205875&amp;lng=16.366904&amp;lib=Wien&amp;url=www.parzival.unibe.ch/hsverz.html#2"]</v>
+        <f t="shared" ref="F4:F67" si="0">"  -  ["&amp;""""&amp;A4&amp;""""&amp;","&amp;""""&amp;"https://heinztschan.github.io/parzival/show_library.html?"&amp;"lat="&amp;D4&amp;"&amp;lng="&amp;E4&amp;"&amp;lib="&amp;B4&amp;"&amp;url=http://"&amp;C4&amp;""""&amp;"]"</f>
+        <v xml:space="preserve">  -  ["Hs. m","https://heinztschan.github.io/parzival/show_library.html?lat=48.205875&amp;lng=16.366904&amp;lib=Wien&amp;url=http://www.parzival.unibe.ch/hsverz.html#2"]</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1180,7 +1180,7 @@
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Hs. n","https://heinztschan.github.io/parzival/show_library.html?lat=49.41914&amp;lng=8.670249&amp;lib=Heidelberg&amp;url=www.parzival.unibe.ch/hsverz.html#3"]</v>
+        <v xml:space="preserve">  -  ["Hs. n","https://heinztschan.github.io/parzival/show_library.html?lat=49.41914&amp;lng=8.670249&amp;lib=Heidelberg&amp;url=http://www.parzival.unibe.ch/hsverz.html#3"]</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Hs. o","https://heinztschan.github.io/parzival/show_library.html?lat=51.028622&amp;lng=13.737017&amp;lib=Dresden&amp;url=www.parzival.unibe.ch/hsverz.html#4"]</v>
+        <v xml:space="preserve">  -  ["Hs. o","https://heinztschan.github.io/parzival/show_library.html?lat=51.028622&amp;lng=13.737017&amp;lib=Dresden&amp;url=http://www.parzival.unibe.ch/hsverz.html#4"]</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1222,7 +1222,7 @@
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Hs. G","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=www.parzival.unibe.ch/hsverz.html#5"]</v>
+        <v xml:space="preserve">  -  ["Hs. G","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#5"]</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Hs. I (Gm)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=www.parzival.unibe.ch/hsverz.html#6"]</v>
+        <v xml:space="preserve">  -  ["Hs. I (Gm)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#6"]</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Hs. L (Gσ)","https://heinztschan.github.io/parzival/show_library.html?lat=53.564724&amp;lng=9.985209&amp;lib=Hamburg&amp;url=www.parzival.unibe.ch/hsverz.html#7"]</v>
+        <v xml:space="preserve">  -  ["Hs. L (Gσ)","https://heinztschan.github.io/parzival/show_library.html?lat=53.564724&amp;lng=9.985209&amp;lib=Hamburg&amp;url=http://www.parzival.unibe.ch/hsverz.html#7"]</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Hs. M (Gυ)","https://heinztschan.github.io/parzival/show_library.html?lat=53.616043&amp;lng=11.414517&amp;lib=Schwerin&amp;url=www.parzival.unibe.ch/hsverz.html#8"]</v>
+        <v xml:space="preserve">  -  ["Hs. M (Gυ)","https://heinztschan.github.io/parzival/show_library.html?lat=53.616043&amp;lng=11.414517&amp;lib=Schwerin&amp;url=http://www.parzival.unibe.ch/hsverz.html#8"]</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1306,7 +1306,7 @@
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Hs. O (Gk)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=www.parzival.unibe.ch/hsverz.html#9"]</v>
+        <v xml:space="preserve">  -  ["Hs. O (Gk)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#9"]</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1327,7 +1327,7 @@
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Hs. Q (Gτ)","https://heinztschan.github.io/parzival/show_library.html?lat=49.00794&amp;lng=8.398618&amp;lib=Karlsruhe&amp;url=www.parzival.unibe.ch/hsverz.html#10"]</v>
+        <v xml:space="preserve">  -  ["Hs. Q (Gτ)","https://heinztschan.github.io/parzival/show_library.html?lat=49.00794&amp;lng=8.398618&amp;lib=Karlsruhe&amp;url=http://www.parzival.unibe.ch/hsverz.html#10"]</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Hs. R (Gχ)","https://heinztschan.github.io/parzival/show_library.html?lat=46.947355&amp;lng=7.44834&amp;lib=Bern&amp;url=www.parzival.unibe.ch/hsverz.html#11"]</v>
+        <v xml:space="preserve">  -  ["Hs. R (Gχ)","https://heinztschan.github.io/parzival/show_library.html?lat=46.947355&amp;lng=7.44834&amp;lib=Bern&amp;url=http://www.parzival.unibe.ch/hsverz.html#11"]</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1369,7 +1369,7 @@
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Hs. T (Gn)","https://heinztschan.github.io/parzival/show_library.html?lat=48.205875&amp;lng=16.366904&amp;lib=Wien&amp;url=www.parzival.unibe.ch/hsverz.html12"]</v>
+        <v xml:space="preserve">  -  ["Hs. T (Gn)","https://heinztschan.github.io/parzival/show_library.html?lat=48.205875&amp;lng=16.366904&amp;lib=Wien&amp;url=http://www.parzival.unibe.ch/hsverz.html12"]</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1390,7 +1390,7 @@
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Hs. U (Gμ)","https://heinztschan.github.io/parzival/show_library.html?lat=48.205875&amp;lng=16.366904&amp;lib=Wien&amp;url=www.parzival.unibe.ch/hsverz.html#13"]</v>
+        <v xml:space="preserve">  -  ["Hs. U (Gμ)","https://heinztschan.github.io/parzival/show_library.html?lat=48.205875&amp;lng=16.366904&amp;lib=Wien&amp;url=http://www.parzival.unibe.ch/hsverz.html#13"]</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Hs. V (Gδ)","https://heinztschan.github.io/parzival/show_library.html?lat=49.00794&amp;lng=8.398618&amp;lib=Karlsruhe&amp;url=www.parzival.unibe.ch/hsverz.html#14"]</v>
+        <v xml:space="preserve">  -  ["Hs. V (Gδ)","https://heinztschan.github.io/parzival/show_library.html?lat=49.00794&amp;lng=8.398618&amp;lib=Karlsruhe&amp;url=http://www.parzival.unibe.ch/hsverz.html#14"]</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1432,7 +1432,7 @@
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Hs. Vʼ (Gδδ)","https://heinztschan.github.io/parzival/show_library.html?lat=41.898825&amp;lng=12.47934&amp;lib=Roma&amp;url=www.parzival.unibe.ch/hsverz.html#15"]</v>
+        <v xml:space="preserve">  -  ["Hs. Vʼ (Gδδ)","https://heinztschan.github.io/parzival/show_library.html?lat=41.898825&amp;lng=12.47934&amp;lib=Roma&amp;url=http://www.parzival.unibe.ch/hsverz.html#15"]</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Druck W (Gφ)","https://heinztschan.github.io/parzival/show_library.html?lat=46.947355&amp;lng=7.44834&amp;lib=Bern&amp;url=www.parzival.unibe.ch/hsverz.html#16"]</v>
+        <v xml:space="preserve">  -  ["Druck W (Gφ)","https://heinztschan.github.io/parzival/show_library.html?lat=46.947355&amp;lng=7.44834&amp;lib=Bern&amp;url=http://www.parzival.unibe.ch/hsverz.html#16"]</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Hs. Z (Gκ)","https://heinztschan.github.io/parzival/show_library.html?lat=49.41914&amp;lng=8.670249&amp;lib=Heidelberg&amp;url=www.parzival.unibe.ch/hsverz.html#17"]</v>
+        <v xml:space="preserve">  -  ["Hs. Z (Gκ)","https://heinztschan.github.io/parzival/show_library.html?lat=49.41914&amp;lng=8.670249&amp;lib=Heidelberg&amp;url=http://www.parzival.unibe.ch/hsverz.html#17"]</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1495,7 +1495,7 @@
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 1 (a)","https://heinztschan.github.io/parzival/show_library.html?lat=48.205875&amp;lng=16.366904&amp;lib=Wien&amp;url=www.parzival.unibe.ch/hsverz.html#18"]</v>
+        <v xml:space="preserve">  -  ["Fr. 1 (a)","https://heinztschan.github.io/parzival/show_library.html?lat=48.205875&amp;lng=16.366904&amp;lib=Wien&amp;url=http://www.parzival.unibe.ch/hsverz.html#18"]</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1516,7 +1516,7 @@
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 2 (b)","https://heinztschan.github.io/parzival/show_library.html?lat=51.528379&amp;lng=11.545036&amp;lib=Eisleben&amp;url=www.parzival.unibe.ch/hsverz.html#19"]</v>
+        <v xml:space="preserve">  -  ["Fr. 2 (b)","https://heinztschan.github.io/parzival/show_library.html?lat=51.528379&amp;lng=11.545036&amp;lib=Eisleben&amp;url=http://www.parzival.unibe.ch/hsverz.html#19"]</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1537,7 +1537,7 @@
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 3 (c )","https://heinztschan.github.io/parzival/show_library.html?lat=50.978516&amp;lng=11.332221&amp;lib=Weimar&amp;url=www.parzival.unibe.ch/hsverz.html#20"]</v>
+        <v xml:space="preserve">  -  ["Fr. 3 (c )","https://heinztschan.github.io/parzival/show_library.html?lat=50.978516&amp;lng=11.332221&amp;lib=Weimar&amp;url=http://www.parzival.unibe.ch/hsverz.html#20"]</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1558,7 +1558,7 @@
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 4 (ç)","https://heinztschan.github.io/parzival/show_library.html?lat=49.751547&amp;lng=6.641294&amp;lib=Trier&amp;url=www.parzival.unibe.ch/hsverz.html#21"]</v>
+        <v xml:space="preserve">  -  ["Fr. 4 (ç)","https://heinztschan.github.io/parzival/show_library.html?lat=49.751547&amp;lng=6.641294&amp;lib=Trier&amp;url=http://www.parzival.unibe.ch/hsverz.html#21"]</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 5 (d)","https://heinztschan.github.io/parzival/show_library.html?lat=47.134889&amp;lng=15.284836&amp;lib=Rein (Steiermark)&amp;url=www.parzival.unibe.ch/hsverz.html#22"]</v>
+        <v xml:space="preserve">  -  ["Fr. 5 (d)","https://heinztschan.github.io/parzival/show_library.html?lat=47.134889&amp;lng=15.284836&amp;lib=Rein (Steiermark)&amp;url=http://www.parzival.unibe.ch/hsverz.html#22"]</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1600,7 +1600,7 @@
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 6 (e)","https://heinztschan.github.io/parzival/show_library.html?lat=53.406773&amp;lng=-2.965723&amp;lib=Liverpool&amp;url=www.parzival.unibe.ch/hsverz.html#23"]</v>
+        <v xml:space="preserve">  -  ["Fr. 6 (e)","https://heinztschan.github.io/parzival/show_library.html?lat=53.406773&amp;lng=-2.965723&amp;lib=Liverpool&amp;url=http://www.parzival.unibe.ch/hsverz.html#23"]</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 7 (f)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=www.parzival.unibe.ch/hsverz.html#24"]</v>
+        <v xml:space="preserve">  -  ["Fr. 7 (f)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#24"]</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1642,7 +1642,7 @@
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 8 (g)","https://heinztschan.github.io/parzival/show_library.html?lat=51.539481&amp;lng=9.935938&amp;lib=Göttingen&amp;url=www.parzival.unibe.ch/hsverz.html#25"]</v>
+        <v xml:space="preserve">  -  ["Fr. 8 (g)","https://heinztschan.github.io/parzival/show_library.html?lat=51.539481&amp;lng=9.935938&amp;lib=Göttingen&amp;url=http://www.parzival.unibe.ch/hsverz.html#25"]</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 9 (h)","https://heinztschan.github.io/parzival/show_library.html?lat=50.945374&amp;lng=10.705386&amp;lib=Gotha&amp;url=www.parzival.unibe.ch/hsverz.html#26"]</v>
+        <v xml:space="preserve">  -  ["Fr. 9 (h)","https://heinztschan.github.io/parzival/show_library.html?lat=50.945374&amp;lng=10.705386&amp;lib=Gotha&amp;url=http://www.parzival.unibe.ch/hsverz.html#26"]</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1684,7 +1684,7 @@
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 9 (h)","https://heinztschan.github.io/parzival/show_library.html?lat=51.372045&amp;lng=10.869609&amp;lib=Sonderhausen&amp;url=www.parzival.unibe.ch/hsverz.html#26"]</v>
+        <v xml:space="preserve">  -  ["Fr. 9 (h)","https://heinztschan.github.io/parzival/show_library.html?lat=51.372045&amp;lng=10.869609&amp;lib=Sonderhausen&amp;url=http://www.parzival.unibe.ch/hsverz.html#26"]</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1705,7 +1705,7 @@
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 10 (i)","https://heinztschan.github.io/parzival/show_library.html?lat=47.074333&amp;lng=15.441019&amp;lib=Graz&amp;url=www.parzival.unibe.ch/hsverz.html#27"]</v>
+        <v xml:space="preserve">  -  ["Fr. 10 (i)","https://heinztschan.github.io/parzival/show_library.html?lat=47.074333&amp;lng=15.441019&amp;lib=Graz&amp;url=http://www.parzival.unibe.ch/hsverz.html#27"]</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1726,7 +1726,7 @@
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 11 (k)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=www.parzival.unibe.ch/hsverz.html#28"]</v>
+        <v xml:space="preserve">  -  ["Fr. 11 (k)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#28"]</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1747,7 +1747,7 @@
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 12 (l)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=www.parzival.unibe.ch/hsverz.html#29"]</v>
+        <v xml:space="preserve">  -  ["Fr. 12 (l)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#29"]</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1768,7 +1768,7 @@
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 13 (ll)","https://heinztschan.github.io/parzival/show_library.html?lat=51.321651&amp;lng=9.505532&amp;lib=Kassel&amp;url=www.parzival.unibe.ch/hsverz.html#30"]</v>
+        <v xml:space="preserve">  -  ["Fr. 13 (ll)","https://heinztschan.github.io/parzival/show_library.html?lat=51.321651&amp;lng=9.505532&amp;lib=Kassel&amp;url=http://www.parzival.unibe.ch/hsverz.html#30"]</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1789,7 +1789,7 @@
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 14 (r)","https://heinztschan.github.io/parzival/show_library.html?lat=49.596704&amp;lng=11.007574&amp;lib=Erlangen&amp;url=www.parzival.unibe.ch/hsverz.html#31"]</v>
+        <v xml:space="preserve">  -  ["Fr. 14 (r)","https://heinztschan.github.io/parzival/show_library.html?lat=49.596704&amp;lng=11.007574&amp;lib=Erlangen&amp;url=http://www.parzival.unibe.ch/hsverz.html#31"]</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1810,7 +1810,7 @@
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 15 (s)","https://heinztschan.github.io/parzival/show_library.html?lat=47.374259&amp;lng=8.545462&amp;lib=Zürich&amp;url=www.parzival.unibe.ch/hsverz.html#32"]</v>
+        <v xml:space="preserve">  -  ["Fr. 15 (s)","https://heinztschan.github.io/parzival/show_library.html?lat=47.374259&amp;lng=8.545462&amp;lib=Zürich&amp;url=http://www.parzival.unibe.ch/hsverz.html#32"]</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1831,7 +1831,7 @@
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 16 (t)","https://heinztschan.github.io/parzival/show_library.html?lat=49.790906&amp;lng=9.934355&amp;lib=Würzburg&amp;url=www.parzival.unibe.ch/hsverz.html#33"]</v>
+        <v xml:space="preserve">  -  ["Fr. 16 (t)","https://heinztschan.github.io/parzival/show_library.html?lat=49.790906&amp;lng=9.934355&amp;lib=Würzburg&amp;url=http://www.parzival.unibe.ch/hsverz.html#33"]</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1852,7 +1852,7 @@
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 17 (E)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=www.parzival.unibe.ch/hsverz.html#34"]</v>
+        <v xml:space="preserve">  -  ["Fr. 17 (E)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#34"]</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1873,7 +1873,7 @@
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 18 (F) ","https://heinztschan.github.io/parzival/show_library.html?lat=48.777241&amp;lng=9.184806&amp;lib=Stuttgart&amp;url=www.parzival.unibe.ch/hsverz.html#35"]</v>
+        <v xml:space="preserve">  -  ["Fr. 18 (F) ","https://heinztschan.github.io/parzival/show_library.html?lat=48.777241&amp;lng=9.184806&amp;lib=Stuttgart&amp;url=http://www.parzival.unibe.ch/hsverz.html#35"]</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1894,7 +1894,7 @@
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 18 (Gl)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=www.parzival.unibe.ch/hsverz.html#35"]</v>
+        <v xml:space="preserve">  -  ["Fr. 18 (Gl)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#35"]</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1915,7 +1915,7 @@
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 18 (Gv)","https://heinztschan.github.io/parzival/show_library.html?lat=49.448249&amp;lng=11.075511&amp;lib=Nürnberg&amp;url=www.parzival.unibe.ch/hsverz.html#35"]</v>
+        <v xml:space="preserve">  -  ["Fr. 18 (Gv)","https://heinztschan.github.io/parzival/show_library.html?lat=49.448249&amp;lng=11.075511&amp;lib=Nürnberg&amp;url=http://www.parzival.unibe.ch/hsverz.html#35"]</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1936,7 +1936,7 @@
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 19 (Ga)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=www.parzival.unibe.ch/hsverz.html#36"]</v>
+        <v xml:space="preserve">  -  ["Fr. 19 (Ga)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#36"]</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1957,7 +1957,7 @@
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 20 (Gb)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=www.parzival.unibe.ch/hsverz.html#37"]</v>
+        <v xml:space="preserve">  -  ["Fr. 20 (Gb)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#37"]</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1978,7 +1978,7 @@
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 21 (Gc)","https://heinztschan.github.io/parzival/show_library.html?lat=48.205875&amp;lng=16.366904&amp;lib=Wien&amp;url=www.parzival.unibe.ch/hsverz.html#38"]</v>
+        <v xml:space="preserve">  -  ["Fr. 21 (Gc)","https://heinztschan.github.io/parzival/show_library.html?lat=48.205875&amp;lng=16.366904&amp;lib=Wien&amp;url=http://www.parzival.unibe.ch/hsverz.html#38"]</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1999,7 +1999,7 @@
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 21 (Gc)","https://heinztschan.github.io/parzival/show_library.html?lat=51.516506&amp;lng=7.460886&amp;lib=Dortmund&amp;url=www.parzival.unibe.ch/hsverz.html#38"]</v>
+        <v xml:space="preserve">  -  ["Fr. 21 (Gc)","https://heinztschan.github.io/parzival/show_library.html?lat=51.516506&amp;lng=7.460886&amp;lib=Dortmund&amp;url=http://www.parzival.unibe.ch/hsverz.html#38"]</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2020,7 +2020,7 @@
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 22 (Gd)","https://heinztschan.github.io/parzival/show_library.html?lat=50.974221&amp;lng=11.022227&amp;lib=Erfurt&amp;url=www.parzival.unibe.ch/hsverz.html#39"]</v>
+        <v xml:space="preserve">  -  ["Fr. 22 (Gd)","https://heinztschan.github.io/parzival/show_library.html?lat=50.974221&amp;lng=11.022227&amp;lib=Erfurt&amp;url=http://www.parzival.unibe.ch/hsverz.html#39"]</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2041,7 +2041,7 @@
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 22 (Gd)","https://heinztschan.github.io/parzival/show_library.html?lat=51.332494&amp;lng=12.368181&amp;lib=Leipzig&amp;url=www.parzival.unibe.ch/hsverz.html#39"]</v>
+        <v xml:space="preserve">  -  ["Fr. 22 (Gd)","https://heinztschan.github.io/parzival/show_library.html?lat=51.332494&amp;lng=12.368181&amp;lib=Leipzig&amp;url=http://www.parzival.unibe.ch/hsverz.html#39"]</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2062,7 +2062,7 @@
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 23 (Ge)","https://heinztschan.github.io/parzival/show_library.html?lat=51.15423&amp;lng=11.80374&amp;lib=Naumburg&amp;url=www.parzival.unibe.ch/hsverz.html#40"]</v>
+        <v xml:space="preserve">  -  ["Fr. 23 (Ge)","https://heinztschan.github.io/parzival/show_library.html?lat=51.15423&amp;lng=11.80374&amp;lib=Naumburg&amp;url=http://www.parzival.unibe.ch/hsverz.html#40"]</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2083,7 +2083,7 @@
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 23 (Ge)","https://heinztschan.github.io/parzival/show_library.html?lat=51.112139&amp;lng=17.050658&amp;lib=Wrocław&amp;url=www.parzival.unibe.ch/hsverz.html#40"]</v>
+        <v xml:space="preserve">  -  ["Fr. 23 (Ge)","https://heinztschan.github.io/parzival/show_library.html?lat=51.112139&amp;lng=17.050658&amp;lib=Wrocław&amp;url=http://www.parzival.unibe.ch/hsverz.html#40"]</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2104,7 +2104,7 @@
       </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 24 (Gf)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=www.parzival.unibe.ch/hsverz.html#41"]</v>
+        <v xml:space="preserve">  -  ["Fr. 24 (Gf)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#41"]</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2125,7 +2125,7 @@
       </c>
       <c r="F50" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 24 (Gf)","https://heinztschan.github.io/parzival/show_library.html?lat=48.562739&amp;lng=16.07229&amp;lib=Oberhollabrunn&amp;url=www.parzival.unibe.ch/hsverz.html#41"]</v>
+        <v xml:space="preserve">  -  ["Fr. 24 (Gf)","https://heinztschan.github.io/parzival/show_library.html?lat=48.562739&amp;lng=16.07229&amp;lib=Oberhollabrunn&amp;url=http://www.parzival.unibe.ch/hsverz.html#41"]</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2146,7 +2146,7 @@
       </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 24 (Gf)","https://heinztschan.github.io/parzival/show_library.html?lat=49.444261&amp;lng=11.850315&amp;lib=Amberg&amp;url=www.parzival.unibe.ch/hsverz.html#41"]</v>
+        <v xml:space="preserve">  -  ["Fr. 24 (Gf)","https://heinztschan.github.io/parzival/show_library.html?lat=49.444261&amp;lng=11.850315&amp;lib=Amberg&amp;url=http://www.parzival.unibe.ch/hsverz.html#41"]</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2167,7 +2167,7 @@
       </c>
       <c r="F52" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 24 (Gf)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=www.parzival.unibe.ch/hsverz.html#41"]</v>
+        <v xml:space="preserve">  -  ["Fr. 24 (Gf)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#41"]</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="F53" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 25 (Gg)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#42"]</v>
+        <v xml:space="preserve">  -  ["Fr. 25 (Gg)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#42"]</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2209,7 +2209,7 @@
       </c>
       <c r="F54" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 26 (Gh)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#43"]</v>
+        <v xml:space="preserve">  -  ["Fr. 26 (Gh)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#43"]</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2230,7 +2230,7 @@
       </c>
       <c r="F55" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 27 (Gi)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#44"]</v>
+        <v xml:space="preserve">  -  ["Fr. 27 (Gi)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#44"]</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2251,7 +2251,7 @@
       </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 28 (Gj)","https://heinztschan.github.io/parzival/show_library.html?lat=50.945374&amp;lng=10.705386&amp;lib=Gotha&amp;url=http://www.parzival.unibe.ch/hsverz.html#45"]</v>
+        <v xml:space="preserve">  -  ["Fr. 28 (Gj)","https://heinztschan.github.io/parzival/show_library.html?lat=50.945374&amp;lng=10.705386&amp;lib=Gotha&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#45"]</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2272,7 +2272,7 @@
       </c>
       <c r="F57" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 28 (Gj)","https://heinztschan.github.io/parzival/show_library.html?lat=51.321651&amp;lng=9.505532&amp;lib=Kassel&amp;url=http://www.parzival.unibe.ch/hsverz.html#45"]</v>
+        <v xml:space="preserve">  -  ["Fr. 28 (Gj)","https://heinztschan.github.io/parzival/show_library.html?lat=51.321651&amp;lng=9.505532&amp;lib=Kassel&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#45"]</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="F58" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 29 (Go)","https://heinztschan.github.io/parzival/show_library.html?lat=49.448249&amp;lng=11.075511&amp;lib=Nürnberg&amp;url=http://www.parzival.unibe.ch/hsverz.html#46"]</v>
+        <v xml:space="preserve">  -  ["Fr. 29 (Go)","https://heinztschan.github.io/parzival/show_library.html?lat=49.448249&amp;lng=11.075511&amp;lib=Nürnberg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#46"]</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2314,7 +2314,7 @@
       </c>
       <c r="F59" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 30 (Gp)","https://heinztschan.github.io/parzival/show_library.html?lat=47.798474&amp;lng=13.047809&amp;lib=Salzburg&amp;url=http://www.parzival.unibe.ch/hsverz.html#47"]</v>
+        <v xml:space="preserve">  -  ["Fr. 30 (Gp)","https://heinztschan.github.io/parzival/show_library.html?lat=47.798474&amp;lng=13.047809&amp;lib=Salzburg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#47"]</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2335,7 +2335,7 @@
       </c>
       <c r="F60" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 31 (Gq)","https://heinztschan.github.io/parzival/show_library.html?lat=47.208828&amp;lng=47.208828&amp;lib=Solothurn&amp;url=http://www.parzival.unibe.ch/hsverz.html#48"]</v>
+        <v xml:space="preserve">  -  ["Fr. 31 (Gq)","https://heinztschan.github.io/parzival/show_library.html?lat=47.208828&amp;lng=47.208828&amp;lib=Solothurn&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#48"]</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2356,7 +2356,7 @@
       </c>
       <c r="F61" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 31 (Gq)","https://heinztschan.github.io/parzival/show_library.html?lat=48.076308&amp;lng=7.361193&amp;lib=Colmar&amp;url=http://www.parzival.unibe.ch/hsverz.html#48"]</v>
+        <v xml:space="preserve">  -  ["Fr. 31 (Gq)","https://heinztschan.github.io/parzival/show_library.html?lat=48.076308&amp;lng=7.361193&amp;lib=Colmar&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#48"]</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2377,7 +2377,7 @@
       </c>
       <c r="F62" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 32 (Gr)","https://heinztschan.github.io/parzival/show_library.html?lat=47.374259&amp;lng=8.545462&amp;lib=Zürich&amp;url=http://www.parzival.unibe.ch/hsverz.html#49"]</v>
+        <v xml:space="preserve">  -  ["Fr. 32 (Gr)","https://heinztschan.github.io/parzival/show_library.html?lat=47.374259&amp;lng=8.545462&amp;lib=Zürich&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#49"]</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2398,7 +2398,7 @@
       </c>
       <c r="F63" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 32 (Gr)","https://heinztschan.github.io/parzival/show_library.html?lat=47.397325&amp;lng=8.547106&amp;lib=Zürich&amp;url=http://www.parzival.unibe.ch/hsverz.html#49"]</v>
+        <v xml:space="preserve">  -  ["Fr. 32 (Gr)","https://heinztschan.github.io/parzival/show_library.html?lat=47.397325&amp;lng=8.547106&amp;lib=Zürich&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#49"]</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2419,7 +2419,7 @@
       </c>
       <c r="F64" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 33 (Gs)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#50"]</v>
+        <v xml:space="preserve">  -  ["Fr. 33 (Gs)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#50"]</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2440,7 +2440,7 @@
       </c>
       <c r="F65" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 34 (Gt)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#51"]</v>
+        <v xml:space="preserve">  -  ["Fr. 34 (Gt)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#51"]</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2461,7 +2461,7 @@
       </c>
       <c r="F66" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 35 (Gu)","https://heinztschan.github.io/parzival/show_library.html?lat=52.164333&amp;lng=10.530299&amp;lib=Wolfenbüttel&amp;url=http://www.parzival.unibe.ch/hsverz.html#52"]</v>
+        <v xml:space="preserve">  -  ["Fr. 35 (Gu)","https://heinztschan.github.io/parzival/show_library.html?lat=52.164333&amp;lng=10.530299&amp;lib=Wolfenbüttel&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#52"]</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2482,7 +2482,7 @@
       </c>
       <c r="F67" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 36 (Gw)","https://heinztschan.github.io/parzival/show_library.html?lat=48.059021&amp;lng=12.233863&amp;lib=Wasserburg&amp;url=http://www.parzival.unibe.ch/hsverz.html#53"]</v>
+        <v xml:space="preserve">  -  ["Fr. 36 (Gw)","https://heinztschan.github.io/parzival/show_library.html?lat=48.059021&amp;lng=12.233863&amp;lib=Wasserburg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#53"]</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2502,8 +2502,8 @@
         <v>9.9359380000000002</v>
       </c>
       <c r="F68" t="str">
-        <f t="shared" ref="F68:F113" si="1">"  -  ["&amp;""""&amp;A68&amp;""""&amp;","&amp;""""&amp;"https://heinztschan.github.io/parzival/show_library.html?"&amp;"lat="&amp;D68&amp;"&amp;lng="&amp;E68&amp;"&amp;lib="&amp;B68&amp;"&amp;url="&amp;C68&amp;""""&amp;"]"</f>
-        <v xml:space="preserve">  -  ["Fr. 37 (Gx)","https://heinztschan.github.io/parzival/show_library.html?lat=51.539481&amp;lng=9.935938&amp;lib=Göttingen&amp;url=http://www.parzival.unibe.ch/hsverz.html#54"]</v>
+        <f t="shared" ref="F68:F113" si="1">"  -  ["&amp;""""&amp;A68&amp;""""&amp;","&amp;""""&amp;"https://heinztschan.github.io/parzival/show_library.html?"&amp;"lat="&amp;D68&amp;"&amp;lng="&amp;E68&amp;"&amp;lib="&amp;B68&amp;"&amp;url=http://"&amp;C68&amp;""""&amp;"]"</f>
+        <v xml:space="preserve">  -  ["Fr. 37 (Gx)","https://heinztschan.github.io/parzival/show_library.html?lat=51.539481&amp;lng=9.935938&amp;lib=Göttingen&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#54"]</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2524,7 +2524,7 @@
       </c>
       <c r="F69" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 38 (Gy)","https://heinztschan.github.io/parzival/show_library.html?lat=49.448249&amp;lng=11.075511&amp;lib=Nürnberg&amp;url=http://www.parzival.unibe.ch/hsverz.html#55"]</v>
+        <v xml:space="preserve">  -  ["Fr. 38 (Gy)","https://heinztschan.github.io/parzival/show_library.html?lat=49.448249&amp;lng=11.075511&amp;lib=Nürnberg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#55"]</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="F70" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 39 (Gz)","https://heinztschan.github.io/parzival/show_library.html?lat=49.448249&amp;lng=11.075511&amp;lib=Nürnberg&amp;url=http://www.parzival.unibe.ch/hsverz.html#56"]</v>
+        <v xml:space="preserve">  -  ["Fr. 39 (Gz)","https://heinztschan.github.io/parzival/show_library.html?lat=49.448249&amp;lng=11.075511&amp;lib=Nürnberg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#56"]</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2566,7 +2566,7 @@
       </c>
       <c r="F71" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 39 (Gπ)","https://heinztschan.github.io/parzival/show_library.html?lat=49.876634&amp;lng=8.657728&amp;lib=Darmstadt&amp;url=http://www.parzival.unibe.ch/hsverz.html#56"]</v>
+        <v xml:space="preserve">  -  ["Fr. 39 (Gπ)","https://heinztschan.github.io/parzival/show_library.html?lat=49.876634&amp;lng=8.657728&amp;lib=Darmstadt&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#56"]</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2587,7 +2587,7 @@
       </c>
       <c r="F72" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 40 (Gα)","https://heinztschan.github.io/parzival/show_library.html?lat=47.34962&amp;lng=11.702285&amp;lib=Schwaz&amp;url=http://www.parzival.unibe.ch/hsverz.html#57"]</v>
+        <v xml:space="preserve">  -  ["Fr. 40 (Gα)","https://heinztschan.github.io/parzival/show_library.html?lat=47.34962&amp;lng=11.702285&amp;lib=Schwaz&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#57"]</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2608,7 +2608,7 @@
       </c>
       <c r="F73" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 40 (Gα)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#57"]</v>
+        <v xml:space="preserve">  -  ["Fr. 40 (Gα)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#57"]</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2629,7 +2629,7 @@
       </c>
       <c r="F74" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 40 (Gα)","https://heinztschan.github.io/parzival/show_library.html?lat=47.074333&amp;lng=15.441019&amp;lib=Graz&amp;url=http://www.parzival.unibe.ch/hsverz.html#57"]</v>
+        <v xml:space="preserve">  -  ["Fr. 40 (Gα)","https://heinztschan.github.io/parzival/show_library.html?lat=47.074333&amp;lng=15.441019&amp;lib=Graz&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#57"]</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2650,7 +2650,7 @@
       </c>
       <c r="F75" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 40 (Gα)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#57"]</v>
+        <v xml:space="preserve">  -  ["Fr. 40 (Gα)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#57"]</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2671,7 +2671,7 @@
       </c>
       <c r="F76" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 41 (Gβ)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#58"]</v>
+        <v xml:space="preserve">  -  ["Fr. 41 (Gβ)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#58"]</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2692,7 +2692,7 @@
       </c>
       <c r="F77" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 42 (Gγ)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#59"]</v>
+        <v xml:space="preserve">  -  ["Fr. 42 (Gγ)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#59"]</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2713,7 +2713,7 @@
       </c>
       <c r="F78" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 43 (Gε)","https://heinztschan.github.io/parzival/show_library.html?lat=51.539481&amp;lng=9.935938&amp;lib=Göttingen&amp;url=http://www.parzival.unibe.ch/hsverz.html#60"]</v>
+        <v xml:space="preserve">  -  ["Fr. 43 (Gε)","https://heinztschan.github.io/parzival/show_library.html?lat=51.539481&amp;lng=9.935938&amp;lib=Göttingen&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#60"]</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2734,7 +2734,7 @@
       </c>
       <c r="F79" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 44 (Gεε)","https://heinztschan.github.io/parzival/show_library.html?lat=48.51989&amp;lng=9.05239&amp;lib=Tübingen&amp;url=http://www.parzival.unibe.ch/hsverz.html#61"]</v>
+        <v xml:space="preserve">  -  ["Fr. 44 (Gεε)","https://heinztschan.github.io/parzival/show_library.html?lat=48.51989&amp;lng=9.05239&amp;lib=Tübingen&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#61"]</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2755,7 +2755,7 @@
       </c>
       <c r="F80" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 45 (Gζ)","https://heinztschan.github.io/parzival/show_library.html?lat=52.214728&amp;lng=7.023893&amp;lib=Borken&amp;url=http://www.parzival.unibe.ch/hsverz.html#62"]</v>
+        <v xml:space="preserve">  -  ["Fr. 45 (Gζ)","https://heinztschan.github.io/parzival/show_library.html?lat=52.214728&amp;lng=7.023893&amp;lib=Borken&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#62"]</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2776,7 +2776,7 @@
       </c>
       <c r="F81" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 45 (Gζ)","https://heinztschan.github.io/parzival/show_library.html?lat=51.962045&amp;lng=7.624984&amp;lib=Münster&amp;url=http://www.parzival.unibe.ch/hsverz.html#62"]</v>
+        <v xml:space="preserve">  -  ["Fr. 45 (Gζ)","https://heinztschan.github.io/parzival/show_library.html?lat=51.962045&amp;lng=7.624984&amp;lib=Münster&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#62"]</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2797,7 +2797,7 @@
       </c>
       <c r="F82" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 46 (Gζζ)","https://heinztschan.github.io/parzival/show_library.html?lat=51.507351&amp;lng=-0.127758&amp;lib=London&amp;url=http://www.parzival.unibe.ch/hsverz.html#63"]</v>
+        <v xml:space="preserve">  -  ["Fr. 46 (Gζζ)","https://heinztschan.github.io/parzival/show_library.html?lat=51.507351&amp;lng=-0.127758&amp;lib=London&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#63"]</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2818,7 +2818,7 @@
       </c>
       <c r="F83" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 47 (Gη)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#64"]</v>
+        <v xml:space="preserve">  -  ["Fr. 47 (Gη)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#64"]</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2839,7 +2839,7 @@
       </c>
       <c r="F84" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 47 (Gη)","https://heinztschan.github.io/parzival/show_library.html?lat=49.3034&amp;lng=10.57451&amp;lib=Ansbach&amp;url=http://www.parzival.unibe.ch/hsverz.html#64"]</v>
+        <v xml:space="preserve">  -  ["Fr. 47 (Gη)","https://heinztschan.github.io/parzival/show_library.html?lat=49.3034&amp;lng=10.57451&amp;lib=Ansbach&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#64"]</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2860,7 +2860,7 @@
       </c>
       <c r="F85" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 48 (Gϑ)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#65"]</v>
+        <v xml:space="preserve">  -  ["Fr. 48 (Gϑ)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#65"]</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2881,7 +2881,7 @@
       </c>
       <c r="F86" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 48 (Gϑ)","https://heinztschan.github.io/parzival/show_library.html?lat=49.448249&amp;lng=11.075511&amp;lib=Nürnberg&amp;url=http://www.parzival.unibe.ch/hsverz.html#65"]</v>
+        <v xml:space="preserve">  -  ["Fr. 48 (Gϑ)","https://heinztschan.github.io/parzival/show_library.html?lat=49.448249&amp;lng=11.075511&amp;lib=Nürnberg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#65"]</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2902,7 +2902,7 @@
       </c>
       <c r="F87" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 48 (Gϑ)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#65"]</v>
+        <v xml:space="preserve">  -  ["Fr. 48 (Gϑ)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#65"]</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2923,7 +2923,7 @@
       </c>
       <c r="F88" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 49 (Gι)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#66"]</v>
+        <v xml:space="preserve">  -  ["Fr. 49 (Gι)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#66"]</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2944,7 +2944,7 @@
       </c>
       <c r="F89" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 50 (Gλ)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#67"]</v>
+        <v xml:space="preserve">  -  ["Fr. 50 (Gλ)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#67"]</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2965,7 +2965,7 @@
       </c>
       <c r="F90" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 50 (Gj)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#67"]</v>
+        <v xml:space="preserve">  -  ["Fr. 50 (Gj)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#67"]</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2986,7 +2986,7 @@
       </c>
       <c r="F91" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 51 (Gν)","https://heinztschan.github.io/parzival/show_library.html?lat=51.964548&amp;lng=7.622206&amp;lib=Münster&amp;url=http://www.parzival.unibe.ch/hsverz.html#68"]</v>
+        <v xml:space="preserve">  -  ["Fr. 51 (Gν)","https://heinztschan.github.io/parzival/show_library.html?lat=51.964548&amp;lng=7.622206&amp;lib=Münster&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#68"]</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -3007,7 +3007,7 @@
       </c>
       <c r="F92" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 51 (Gω)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#68"]</v>
+        <v xml:space="preserve">  -  ["Fr. 51 (Gω)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#68"]</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -3028,7 +3028,7 @@
       </c>
       <c r="F93" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 52 (Gξ)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#69"]</v>
+        <v xml:space="preserve">  -  ["Fr. 52 (Gξ)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#69"]</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="F94" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 53 (Gρ)","https://heinztschan.github.io/parzival/show_library.html?lat=50.086615&amp;lng=14.415983&amp;lib=Praha&amp;url=http://www.parzival.unibe.ch/hsverz.html#70"]</v>
+        <v xml:space="preserve">  -  ["Fr. 53 (Gρ)","https://heinztschan.github.io/parzival/show_library.html?lat=50.086615&amp;lng=14.415983&amp;lib=Praha&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#70"]</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -3070,7 +3070,7 @@
       </c>
       <c r="F95" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 54 (Gψ)","https://heinztschan.github.io/parzival/show_library.html?lat=47.994248&amp;lng=7.845004&amp;lib=Freiburg i. Br.&amp;url=http://www.parzival.unibe.ch/hsverz.html#71"]</v>
+        <v xml:space="preserve">  -  ["Fr. 54 (Gψ)","https://heinztschan.github.io/parzival/show_library.html?lat=47.994248&amp;lng=7.845004&amp;lib=Freiburg i. Br.&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#71"]</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -3091,7 +3091,7 @@
       </c>
       <c r="F96" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 55 (B)","https://heinztschan.github.io/parzival/show_library.html?lat=48.205875&amp;lng=16.366904&amp;lib=Wien&amp;url=http://www.parzival.unibe.ch/hsverz.html#72"]</v>
+        <v xml:space="preserve">  -  ["Fr. 55 (B)","https://heinztschan.github.io/parzival/show_library.html?lat=48.205875&amp;lng=16.366904&amp;lib=Wien&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#72"]</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -3112,7 +3112,7 @@
       </c>
       <c r="F97" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 56 (C )","https://heinztschan.github.io/parzival/show_library.html?lat=48.297264&amp;lng=14.290971&amp;lib=Linz&amp;url=http://www.parzival.unibe.ch/hsverz.html#73"]</v>
+        <v xml:space="preserve">  -  ["Fr. 56 (C )","https://heinztschan.github.io/parzival/show_library.html?lat=48.297264&amp;lng=14.290971&amp;lib=Linz&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#73"]</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -3133,7 +3133,7 @@
       </c>
       <c r="F98" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 57 (H)","https://heinztschan.github.io/parzival/show_library.html?lat=49.403415&amp;lng=8.675165&amp;lib=Heidelberg&amp;url=http://www.parzival.unibe.ch/hsverz.html#74"]</v>
+        <v xml:space="preserve">  -  ["Fr. 57 (H)","https://heinztschan.github.io/parzival/show_library.html?lat=49.403415&amp;lng=8.675165&amp;lib=Heidelberg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#74"]</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -3154,7 +3154,7 @@
       </c>
       <c r="F99" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 58 (q)","https://heinztschan.github.io/parzival/show_library.html?lat=47.994248&amp;lng=7.845004&amp;lib=Freiburg i. Br.&amp;url=http://www.parzival.unibe.ch/hsverz.html#75"]</v>
+        <v xml:space="preserve">  -  ["Fr. 58 (q)","https://heinztschan.github.io/parzival/show_library.html?lat=47.994248&amp;lng=7.845004&amp;lib=Freiburg i. Br.&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#75"]</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -3175,7 +3175,7 @@
       </c>
       <c r="F100" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 59","https://heinztschan.github.io/parzival/show_library.html?lat=50.80355&amp;lng=8.76291&amp;lib=Marburg&amp;url=http://www.parzival.unibe.ch/hsverz.html#76"]</v>
+        <v xml:space="preserve">  -  ["Fr. 59","https://heinztschan.github.io/parzival/show_library.html?lat=50.80355&amp;lng=8.76291&amp;lib=Marburg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#76"]</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -3196,7 +3196,7 @@
       </c>
       <c r="F101" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 60","https://heinztschan.github.io/parzival/show_library.html?lat=46.04752&amp;lng=14.503967&amp;lib=Ljubljana&amp;url=http://www.parzival.unibe.ch/hsverz.html#77"]</v>
+        <v xml:space="preserve">  -  ["Fr. 60","https://heinztschan.github.io/parzival/show_library.html?lat=46.04752&amp;lng=14.503967&amp;lib=Ljubljana&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#77"]</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -3217,7 +3217,7 @@
       </c>
       <c r="F102" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 61","https://heinztschan.github.io/parzival/show_library.html?lat=49.403415&amp;lng=8.675165&amp;lib=Heidelberg&amp;url=http://www.parzival.unibe.ch/hsverz.html#78"]</v>
+        <v xml:space="preserve">  -  ["Fr. 61","https://heinztschan.github.io/parzival/show_library.html?lat=49.403415&amp;lng=8.675165&amp;lib=Heidelberg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#78"]</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -3238,7 +3238,7 @@
       </c>
       <c r="F103" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 62","https://heinztschan.github.io/parzival/show_library.html?lat=53.20348&amp;lng=5.790048&amp;lib=Leeuwarden&amp;url=http://www.parzival.unibe.ch/hsverz.html#79"]</v>
+        <v xml:space="preserve">  -  ["Fr. 62","https://heinztschan.github.io/parzival/show_library.html?lat=53.20348&amp;lng=5.790048&amp;lib=Leeuwarden&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#79"]</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -3259,7 +3259,7 @@
       </c>
       <c r="F104" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 63","https://heinztschan.github.io/parzival/show_library.html?lat=48.213185&amp;lng=16.36005&amp;lib=Wien&amp;url=http://www.parzival.unibe.ch/hsverz.html#80"]</v>
+        <v xml:space="preserve">  -  ["Fr. 63","https://heinztschan.github.io/parzival/show_library.html?lat=48.213185&amp;lng=16.36005&amp;lib=Wien&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#80"]</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -3280,7 +3280,7 @@
       </c>
       <c r="F105" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 64","https://heinztschan.github.io/parzival/show_library.html?lat=51.366239&amp;lng=8.989292&amp;lib=Mengeringhausen&amp;url=http://www.parzival.unibe.ch/hsverz.html#81"]</v>
+        <v xml:space="preserve">  -  ["Fr. 64","https://heinztschan.github.io/parzival/show_library.html?lat=51.366239&amp;lng=8.989292&amp;lib=Mengeringhausen&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#81"]</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -3301,7 +3301,7 @@
       </c>
       <c r="F106" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 65","https://heinztschan.github.io/parzival/show_library.html?lat=52.369504&amp;lng=9.730706&amp;lib=Hannover&amp;url=http://www.parzival.unibe.ch/hsverz.html#82"]</v>
+        <v xml:space="preserve">  -  ["Fr. 65","https://heinztschan.github.io/parzival/show_library.html?lat=52.369504&amp;lng=9.730706&amp;lib=Hannover&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#82"]</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -3322,7 +3322,7 @@
       </c>
       <c r="F107" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 66","https://heinztschan.github.io/parzival/show_library.html?lat=48.33454&amp;lng=10.895091&amp;lib=Augsburg&amp;url=http://www.parzival.unibe.ch/hsverz.html#83"]</v>
+        <v xml:space="preserve">  -  ["Fr. 66","https://heinztschan.github.io/parzival/show_library.html?lat=48.33454&amp;lng=10.895091&amp;lib=Augsburg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#83"]</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -3343,7 +3343,7 @@
       </c>
       <c r="F108" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 67","https://heinztschan.github.io/parzival/show_library.html?lat=48.79763&amp;lng=9.2251&amp;lib=Stuttgart&amp;url=http://www.parzival.unibe.ch/hsverz.html#84"]</v>
+        <v xml:space="preserve">  -  ["Fr. 67","https://heinztschan.github.io/parzival/show_library.html?lat=48.79763&amp;lng=9.2251&amp;lib=Stuttgart&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#84"]</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -3364,7 +3364,7 @@
       </c>
       <c r="F109" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 68","https://heinztschan.github.io/parzival/show_library.html?lat=51.844647&amp;lng=6.427598&amp;lib=Schloss Anholt&amp;url=http://www.parzival.unibe.ch/hsverz.html#85"]</v>
+        <v xml:space="preserve">  -  ["Fr. 68","https://heinztschan.github.io/parzival/show_library.html?lat=51.844647&amp;lng=6.427598&amp;lib=Schloss Anholt&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#85"]</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -3385,7 +3385,7 @@
       </c>
       <c r="F110" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 68","https://heinztschan.github.io/parzival/show_library.html?lat=50.937531&amp;lng=6.960279&amp;lib=Köln&amp;url=http://www.parzival.unibe.ch/hsverz.html#85"]</v>
+        <v xml:space="preserve">  -  ["Fr. 68","https://heinztschan.github.io/parzival/show_library.html?lat=50.937531&amp;lng=6.960279&amp;lib=Köln&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#85"]</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -3406,7 +3406,7 @@
       </c>
       <c r="F111" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 69","https://heinztschan.github.io/parzival/show_library.html?lat=47.208828&amp;lng=7.532055&amp;lib=Solothurn&amp;url=http://www.parzival.unibe.ch/hsverz.html#86"]</v>
+        <v xml:space="preserve">  -  ["Fr. 69","https://heinztschan.github.io/parzival/show_library.html?lat=47.208828&amp;lng=7.532055&amp;lib=Solothurn&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#86"]</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -3427,7 +3427,7 @@
       </c>
       <c r="F112" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 70","https://heinztschan.github.io/parzival/show_library.html?lat=51.980564&amp;lng=5.904767&amp;lib=Arnhem&amp;url=http://www.parzival.unibe.ch/hsverz.html87"]</v>
+        <v xml:space="preserve">  -  ["Fr. 70","https://heinztschan.github.io/parzival/show_library.html?lat=51.980564&amp;lng=5.904767&amp;lib=Arnhem&amp;url=http://http://www.parzival.unibe.ch/hsverz.html87"]</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -3448,7 +3448,7 @@
       </c>
       <c r="F113" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 71","https://heinztschan.github.io/parzival/show_library.html?lat=50.079951&amp;lng=14.431825&amp;lib=Praha&amp;url=http://www.parzival.unibe.ch/hsverz.html#88"]</v>
+        <v xml:space="preserve">  -  ["Fr. 71","https://heinztschan.github.io/parzival/show_library.html?lat=50.079951&amp;lng=14.431825&amp;lib=Praha&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#88"]</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fehler manchmal mit manchmal ohne http korrigiert
</commit_message>
<xml_diff>
--- a/Parzival_Daten_für_manuscripts.yml.xlsx
+++ b/Parzival_Daten_für_manuscripts.yml.xlsx
@@ -617,148 +617,148 @@
     <t>www.parzival.unibe.ch/hsverz.html#41</t>
   </si>
   <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#42</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#43</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#44</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#45</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#46</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#47</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#48</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#49</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#50</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#51</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#52</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#53</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#54</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#55</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#56</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#57</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#58</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#59</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#60</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#61</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#62</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#63</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#64</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#65</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#66</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#67</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#68</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#69</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#70</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#71</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#72</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#73</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#74</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#75</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#76</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#77</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#78</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#79</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#80</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#81</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#82</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#83</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#84</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#85</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#86</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html87</t>
-  </si>
-  <si>
-    <t>http://www.parzival.unibe.ch/hsverz.html#88</t>
-  </si>
-  <si>
     <t>Parameter für manuscripts.yml</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#42</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#43</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#44</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#45</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#46</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#47</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#48</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#49</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#50</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#51</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#52</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#53</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#54</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#55</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#56</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#57</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#58</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#59</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#60</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#61</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#62</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#63</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#64</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#65</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#66</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#67</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#68</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#69</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#70</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#71</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#72</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#73</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#74</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#75</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#76</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#77</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#78</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#79</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#80</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#81</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#82</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#83</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#84</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#85</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#86</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html87</t>
+  </si>
+  <si>
+    <t>www.parzival.unibe.ch/hsverz.html#88</t>
   </si>
 </sst>
 </file>
@@ -1090,13 +1090,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C90" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
       <selection activeCell="F3" sqref="F3:F113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="27" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="87.75" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1117,7 +1117,7 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>243</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2178,7 +2178,7 @@
         <v>42</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D53">
         <v>52.507599999999996</v>
@@ -2188,7 +2188,7 @@
       </c>
       <c r="F53" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 25 (Gg)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#42"]</v>
+        <v xml:space="preserve">  -  ["Fr. 25 (Gg)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#42"]</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2199,7 +2199,7 @@
         <v>11</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D54">
         <v>48.147409000000003</v>
@@ -2209,7 +2209,7 @@
       </c>
       <c r="F54" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 26 (Gh)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#43"]</v>
+        <v xml:space="preserve">  -  ["Fr. 26 (Gh)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#43"]</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2220,7 +2220,7 @@
         <v>11</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D55">
         <v>48.147409000000003</v>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="F55" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 27 (Gi)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#44"]</v>
+        <v xml:space="preserve">  -  ["Fr. 27 (Gi)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#44"]</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2241,7 +2241,7 @@
         <v>46</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D56">
         <v>50.945374000000001</v>
@@ -2251,7 +2251,7 @@
       </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 28 (Gj)","https://heinztschan.github.io/parzival/show_library.html?lat=50.945374&amp;lng=10.705386&amp;lib=Gotha&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#45"]</v>
+        <v xml:space="preserve">  -  ["Fr. 28 (Gj)","https://heinztschan.github.io/parzival/show_library.html?lat=50.945374&amp;lng=10.705386&amp;lib=Gotha&amp;url=http://www.parzival.unibe.ch/hsverz.html#45"]</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2262,7 +2262,7 @@
         <v>53</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D57">
         <v>51.321651000000003</v>
@@ -2272,7 +2272,7 @@
       </c>
       <c r="F57" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 28 (Gj)","https://heinztschan.github.io/parzival/show_library.html?lat=51.321651&amp;lng=9.505532&amp;lib=Kassel&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#45"]</v>
+        <v xml:space="preserve">  -  ["Fr. 28 (Gj)","https://heinztschan.github.io/parzival/show_library.html?lat=51.321651&amp;lng=9.505532&amp;lib=Kassel&amp;url=http://www.parzival.unibe.ch/hsverz.html#45"]</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2283,7 +2283,7 @@
         <v>65</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D58">
         <v>49.448248999999997</v>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="F58" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 29 (Go)","https://heinztschan.github.io/parzival/show_library.html?lat=49.448249&amp;lng=11.075511&amp;lib=Nürnberg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#46"]</v>
+        <v xml:space="preserve">  -  ["Fr. 29 (Go)","https://heinztschan.github.io/parzival/show_library.html?lat=49.448249&amp;lng=11.075511&amp;lib=Nürnberg&amp;url=http://www.parzival.unibe.ch/hsverz.html#46"]</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2304,7 +2304,7 @@
         <v>86</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D59">
         <v>47.798473999999999</v>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="F59" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 30 (Gp)","https://heinztschan.github.io/parzival/show_library.html?lat=47.798474&amp;lng=13.047809&amp;lib=Salzburg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#47"]</v>
+        <v xml:space="preserve">  -  ["Fr. 30 (Gp)","https://heinztschan.github.io/parzival/show_library.html?lat=47.798474&amp;lng=13.047809&amp;lib=Salzburg&amp;url=http://www.parzival.unibe.ch/hsverz.html#47"]</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2325,7 +2325,7 @@
         <v>88</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D60">
         <v>47.208827999999997</v>
@@ -2335,7 +2335,7 @@
       </c>
       <c r="F60" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 31 (Gq)","https://heinztschan.github.io/parzival/show_library.html?lat=47.208828&amp;lng=47.208828&amp;lib=Solothurn&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#48"]</v>
+        <v xml:space="preserve">  -  ["Fr. 31 (Gq)","https://heinztschan.github.io/parzival/show_library.html?lat=47.208828&amp;lng=47.208828&amp;lib=Solothurn&amp;url=http://www.parzival.unibe.ch/hsverz.html#48"]</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2346,7 +2346,7 @@
         <v>89</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D61">
         <v>48.076307999999997</v>
@@ -2356,7 +2356,7 @@
       </c>
       <c r="F61" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 31 (Gq)","https://heinztschan.github.io/parzival/show_library.html?lat=48.076308&amp;lng=7.361193&amp;lib=Colmar&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#48"]</v>
+        <v xml:space="preserve">  -  ["Fr. 31 (Gq)","https://heinztschan.github.io/parzival/show_library.html?lat=48.076308&amp;lng=7.361193&amp;lib=Colmar&amp;url=http://www.parzival.unibe.ch/hsverz.html#48"]</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2367,7 +2367,7 @@
         <v>57</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D62">
         <v>47.374259000000002</v>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="F62" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 32 (Gr)","https://heinztschan.github.io/parzival/show_library.html?lat=47.374259&amp;lng=8.545462&amp;lib=Zürich&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#49"]</v>
+        <v xml:space="preserve">  -  ["Fr. 32 (Gr)","https://heinztschan.github.io/parzival/show_library.html?lat=47.374259&amp;lng=8.545462&amp;lib=Zürich&amp;url=http://www.parzival.unibe.ch/hsverz.html#49"]</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2388,7 +2388,7 @@
         <v>57</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D63">
         <v>47.397325000000002</v>
@@ -2398,7 +2398,7 @@
       </c>
       <c r="F63" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 32 (Gr)","https://heinztschan.github.io/parzival/show_library.html?lat=47.397325&amp;lng=8.547106&amp;lib=Zürich&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#49"]</v>
+        <v xml:space="preserve">  -  ["Fr. 32 (Gr)","https://heinztschan.github.io/parzival/show_library.html?lat=47.397325&amp;lng=8.547106&amp;lib=Zürich&amp;url=http://www.parzival.unibe.ch/hsverz.html#49"]</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2409,7 +2409,7 @@
         <v>42</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D64">
         <v>52.507599999999996</v>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="F64" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 33 (Gs)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#50"]</v>
+        <v xml:space="preserve">  -  ["Fr. 33 (Gs)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#50"]</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2430,7 +2430,7 @@
         <v>11</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D65">
         <v>48.147409000000003</v>
@@ -2440,7 +2440,7 @@
       </c>
       <c r="F65" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 34 (Gt)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#51"]</v>
+        <v xml:space="preserve">  -  ["Fr. 34 (Gt)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#51"]</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2451,7 +2451,7 @@
         <v>94</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D66">
         <v>52.164332999999999</v>
@@ -2461,7 +2461,7 @@
       </c>
       <c r="F66" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 35 (Gu)","https://heinztschan.github.io/parzival/show_library.html?lat=52.164333&amp;lng=10.530299&amp;lib=Wolfenbüttel&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#52"]</v>
+        <v xml:space="preserve">  -  ["Fr. 35 (Gu)","https://heinztschan.github.io/parzival/show_library.html?lat=52.164333&amp;lng=10.530299&amp;lib=Wolfenbüttel&amp;url=http://www.parzival.unibe.ch/hsverz.html#52"]</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2472,7 +2472,7 @@
         <v>96</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D67">
         <v>48.059021000000001</v>
@@ -2482,7 +2482,7 @@
       </c>
       <c r="F67" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  -  ["Fr. 36 (Gw)","https://heinztschan.github.io/parzival/show_library.html?lat=48.059021&amp;lng=12.233863&amp;lib=Wasserburg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#53"]</v>
+        <v xml:space="preserve">  -  ["Fr. 36 (Gw)","https://heinztschan.github.io/parzival/show_library.html?lat=48.059021&amp;lng=12.233863&amp;lib=Wasserburg&amp;url=http://www.parzival.unibe.ch/hsverz.html#53"]</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2493,7 +2493,7 @@
         <v>44</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D68">
         <v>51.539481000000002</v>
@@ -2503,7 +2503,7 @@
       </c>
       <c r="F68" t="str">
         <f t="shared" ref="F68:F113" si="1">"  -  ["&amp;""""&amp;A68&amp;""""&amp;","&amp;""""&amp;"https://heinztschan.github.io/parzival/show_library.html?"&amp;"lat="&amp;D68&amp;"&amp;lng="&amp;E68&amp;"&amp;lib="&amp;B68&amp;"&amp;url=http://"&amp;C68&amp;""""&amp;"]"</f>
-        <v xml:space="preserve">  -  ["Fr. 37 (Gx)","https://heinztschan.github.io/parzival/show_library.html?lat=51.539481&amp;lng=9.935938&amp;lib=Göttingen&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#54"]</v>
+        <v xml:space="preserve">  -  ["Fr. 37 (Gx)","https://heinztschan.github.io/parzival/show_library.html?lat=51.539481&amp;lng=9.935938&amp;lib=Göttingen&amp;url=http://www.parzival.unibe.ch/hsverz.html#54"]</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2514,7 +2514,7 @@
         <v>65</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D69">
         <v>49.448248999999997</v>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="F69" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 38 (Gy)","https://heinztschan.github.io/parzival/show_library.html?lat=49.448249&amp;lng=11.075511&amp;lib=Nürnberg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#55"]</v>
+        <v xml:space="preserve">  -  ["Fr. 38 (Gy)","https://heinztschan.github.io/parzival/show_library.html?lat=49.448249&amp;lng=11.075511&amp;lib=Nürnberg&amp;url=http://www.parzival.unibe.ch/hsverz.html#55"]</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2535,7 +2535,7 @@
         <v>65</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D70">
         <v>49.448248999999997</v>
@@ -2545,7 +2545,7 @@
       </c>
       <c r="F70" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 39 (Gz)","https://heinztschan.github.io/parzival/show_library.html?lat=49.448249&amp;lng=11.075511&amp;lib=Nürnberg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#56"]</v>
+        <v xml:space="preserve">  -  ["Fr. 39 (Gz)","https://heinztschan.github.io/parzival/show_library.html?lat=49.448249&amp;lng=11.075511&amp;lib=Nürnberg&amp;url=http://www.parzival.unibe.ch/hsverz.html#56"]</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2556,7 +2556,7 @@
         <v>101</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D71">
         <v>49.876634000000003</v>
@@ -2566,7 +2566,7 @@
       </c>
       <c r="F71" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 39 (Gπ)","https://heinztschan.github.io/parzival/show_library.html?lat=49.876634&amp;lng=8.657728&amp;lib=Darmstadt&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#56"]</v>
+        <v xml:space="preserve">  -  ["Fr. 39 (Gπ)","https://heinztschan.github.io/parzival/show_library.html?lat=49.876634&amp;lng=8.657728&amp;lib=Darmstadt&amp;url=http://www.parzival.unibe.ch/hsverz.html#56"]</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2577,7 +2577,7 @@
         <v>103</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D72">
         <v>47.349620000000002</v>
@@ -2587,7 +2587,7 @@
       </c>
       <c r="F72" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 40 (Gα)","https://heinztschan.github.io/parzival/show_library.html?lat=47.34962&amp;lng=11.702285&amp;lib=Schwaz&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#57"]</v>
+        <v xml:space="preserve">  -  ["Fr. 40 (Gα)","https://heinztschan.github.io/parzival/show_library.html?lat=47.34962&amp;lng=11.702285&amp;lib=Schwaz&amp;url=http://www.parzival.unibe.ch/hsverz.html#57"]</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2598,7 +2598,7 @@
         <v>42</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D73">
         <v>52.507599999999996</v>
@@ -2608,7 +2608,7 @@
       </c>
       <c r="F73" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 40 (Gα)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#57"]</v>
+        <v xml:space="preserve">  -  ["Fr. 40 (Gα)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#57"]</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2619,7 +2619,7 @@
         <v>49</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D74">
         <v>47.074333000000003</v>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="F74" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 40 (Gα)","https://heinztschan.github.io/parzival/show_library.html?lat=47.074333&amp;lng=15.441019&amp;lib=Graz&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#57"]</v>
+        <v xml:space="preserve">  -  ["Fr. 40 (Gα)","https://heinztschan.github.io/parzival/show_library.html?lat=47.074333&amp;lng=15.441019&amp;lib=Graz&amp;url=http://www.parzival.unibe.ch/hsverz.html#57"]</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2640,7 +2640,7 @@
         <v>11</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D75">
         <v>48.147409000000003</v>
@@ -2650,7 +2650,7 @@
       </c>
       <c r="F75" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 40 (Gα)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#57"]</v>
+        <v xml:space="preserve">  -  ["Fr. 40 (Gα)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#57"]</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2661,7 +2661,7 @@
         <v>11</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D76">
         <v>48.147409000000003</v>
@@ -2671,7 +2671,7 @@
       </c>
       <c r="F76" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 41 (Gβ)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#58"]</v>
+        <v xml:space="preserve">  -  ["Fr. 41 (Gβ)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#58"]</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2682,7 +2682,7 @@
         <v>11</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D77">
         <v>48.147409000000003</v>
@@ -2692,7 +2692,7 @@
       </c>
       <c r="F77" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 42 (Gγ)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#59"]</v>
+        <v xml:space="preserve">  -  ["Fr. 42 (Gγ)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#59"]</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2703,7 +2703,7 @@
         <v>44</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D78">
         <v>51.539481000000002</v>
@@ -2713,7 +2713,7 @@
       </c>
       <c r="F78" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 43 (Gε)","https://heinztschan.github.io/parzival/show_library.html?lat=51.539481&amp;lng=9.935938&amp;lib=Göttingen&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#60"]</v>
+        <v xml:space="preserve">  -  ["Fr. 43 (Gε)","https://heinztschan.github.io/parzival/show_library.html?lat=51.539481&amp;lng=9.935938&amp;lib=Göttingen&amp;url=http://www.parzival.unibe.ch/hsverz.html#60"]</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2724,7 +2724,7 @@
         <v>109</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D79">
         <v>48.519889999999997</v>
@@ -2734,7 +2734,7 @@
       </c>
       <c r="F79" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 44 (Gεε)","https://heinztschan.github.io/parzival/show_library.html?lat=48.51989&amp;lng=9.05239&amp;lib=Tübingen&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#61"]</v>
+        <v xml:space="preserve">  -  ["Fr. 44 (Gεε)","https://heinztschan.github.io/parzival/show_library.html?lat=48.51989&amp;lng=9.05239&amp;lib=Tübingen&amp;url=http://www.parzival.unibe.ch/hsverz.html#61"]</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2745,7 +2745,7 @@
         <v>111</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D80">
         <v>52.214728000000001</v>
@@ -2755,7 +2755,7 @@
       </c>
       <c r="F80" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 45 (Gζ)","https://heinztschan.github.io/parzival/show_library.html?lat=52.214728&amp;lng=7.023893&amp;lib=Borken&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#62"]</v>
+        <v xml:space="preserve">  -  ["Fr. 45 (Gζ)","https://heinztschan.github.io/parzival/show_library.html?lat=52.214728&amp;lng=7.023893&amp;lib=Borken&amp;url=http://www.parzival.unibe.ch/hsverz.html#62"]</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2766,7 +2766,7 @@
         <v>113</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D81">
         <v>51.962045000000003</v>
@@ -2776,7 +2776,7 @@
       </c>
       <c r="F81" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 45 (Gζ)","https://heinztschan.github.io/parzival/show_library.html?lat=51.962045&amp;lng=7.624984&amp;lib=Münster&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#62"]</v>
+        <v xml:space="preserve">  -  ["Fr. 45 (Gζ)","https://heinztschan.github.io/parzival/show_library.html?lat=51.962045&amp;lng=7.624984&amp;lib=Münster&amp;url=http://www.parzival.unibe.ch/hsverz.html#62"]</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2787,7 +2787,7 @@
         <v>114</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D82">
         <v>51.507351</v>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="F82" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 46 (Gζζ)","https://heinztschan.github.io/parzival/show_library.html?lat=51.507351&amp;lng=-0.127758&amp;lib=London&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#63"]</v>
+        <v xml:space="preserve">  -  ["Fr. 46 (Gζζ)","https://heinztschan.github.io/parzival/show_library.html?lat=51.507351&amp;lng=-0.127758&amp;lib=London&amp;url=http://www.parzival.unibe.ch/hsverz.html#63"]</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2808,7 +2808,7 @@
         <v>42</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D83">
         <v>52.507599999999996</v>
@@ -2818,7 +2818,7 @@
       </c>
       <c r="F83" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 47 (Gη)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#64"]</v>
+        <v xml:space="preserve">  -  ["Fr. 47 (Gη)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#64"]</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2829,7 +2829,7 @@
         <v>116</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D84">
         <v>49.303400000000003</v>
@@ -2839,7 +2839,7 @@
       </c>
       <c r="F84" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 47 (Gη)","https://heinztschan.github.io/parzival/show_library.html?lat=49.3034&amp;lng=10.57451&amp;lib=Ansbach&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#64"]</v>
+        <v xml:space="preserve">  -  ["Fr. 47 (Gη)","https://heinztschan.github.io/parzival/show_library.html?lat=49.3034&amp;lng=10.57451&amp;lib=Ansbach&amp;url=http://www.parzival.unibe.ch/hsverz.html#64"]</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2850,7 +2850,7 @@
         <v>11</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D85">
         <v>48.147409000000003</v>
@@ -2860,7 +2860,7 @@
       </c>
       <c r="F85" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 48 (Gϑ)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#65"]</v>
+        <v xml:space="preserve">  -  ["Fr. 48 (Gϑ)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#65"]</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2871,7 +2871,7 @@
         <v>65</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D86">
         <v>49.448248999999997</v>
@@ -2881,7 +2881,7 @@
       </c>
       <c r="F86" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 48 (Gϑ)","https://heinztschan.github.io/parzival/show_library.html?lat=49.448249&amp;lng=11.075511&amp;lib=Nürnberg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#65"]</v>
+        <v xml:space="preserve">  -  ["Fr. 48 (Gϑ)","https://heinztschan.github.io/parzival/show_library.html?lat=49.448249&amp;lng=11.075511&amp;lib=Nürnberg&amp;url=http://www.parzival.unibe.ch/hsverz.html#65"]</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2892,7 +2892,7 @@
         <v>42</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D87">
         <v>52.507599999999996</v>
@@ -2902,7 +2902,7 @@
       </c>
       <c r="F87" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 48 (Gϑ)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#65"]</v>
+        <v xml:space="preserve">  -  ["Fr. 48 (Gϑ)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#65"]</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2913,7 +2913,7 @@
         <v>42</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D88">
         <v>52.507599999999996</v>
@@ -2923,7 +2923,7 @@
       </c>
       <c r="F88" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 49 (Gι)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#66"]</v>
+        <v xml:space="preserve">  -  ["Fr. 49 (Gι)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#66"]</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2934,7 +2934,7 @@
         <v>11</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D89">
         <v>48.147409000000003</v>
@@ -2944,7 +2944,7 @@
       </c>
       <c r="F89" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 50 (Gλ)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#67"]</v>
+        <v xml:space="preserve">  -  ["Fr. 50 (Gλ)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#67"]</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2955,7 +2955,7 @@
         <v>11</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D90">
         <v>48.147409000000003</v>
@@ -2965,7 +2965,7 @@
       </c>
       <c r="F90" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 50 (Gj)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#67"]</v>
+        <v xml:space="preserve">  -  ["Fr. 50 (Gj)","https://heinztschan.github.io/parzival/show_library.html?lat=48.147409&amp;lng=11.580612&amp;lib=München&amp;url=http://www.parzival.unibe.ch/hsverz.html#67"]</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2976,7 +2976,7 @@
         <v>113</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D91">
         <v>51.964548000000001</v>
@@ -2986,7 +2986,7 @@
       </c>
       <c r="F91" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 51 (Gν)","https://heinztschan.github.io/parzival/show_library.html?lat=51.964548&amp;lng=7.622206&amp;lib=Münster&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#68"]</v>
+        <v xml:space="preserve">  -  ["Fr. 51 (Gν)","https://heinztschan.github.io/parzival/show_library.html?lat=51.964548&amp;lng=7.622206&amp;lib=Münster&amp;url=http://www.parzival.unibe.ch/hsverz.html#68"]</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2997,7 +2997,7 @@
         <v>42</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D92">
         <v>52.507599999999996</v>
@@ -3007,7 +3007,7 @@
       </c>
       <c r="F92" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 51 (Gω)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#68"]</v>
+        <v xml:space="preserve">  -  ["Fr. 51 (Gω)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#68"]</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -3018,7 +3018,7 @@
         <v>42</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D93">
         <v>52.507599999999996</v>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="F93" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 52 (Gξ)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#69"]</v>
+        <v xml:space="preserve">  -  ["Fr. 52 (Gξ)","https://heinztschan.github.io/parzival/show_library.html?lat=52.5076&amp;lng=13.370814&amp;lib=Berlin&amp;url=http://www.parzival.unibe.ch/hsverz.html#69"]</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -3039,7 +3039,7 @@
         <v>125</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D94">
         <v>50.086615000000002</v>
@@ -3049,7 +3049,7 @@
       </c>
       <c r="F94" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 53 (Gρ)","https://heinztschan.github.io/parzival/show_library.html?lat=50.086615&amp;lng=14.415983&amp;lib=Praha&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#70"]</v>
+        <v xml:space="preserve">  -  ["Fr. 53 (Gρ)","https://heinztschan.github.io/parzival/show_library.html?lat=50.086615&amp;lng=14.415983&amp;lib=Praha&amp;url=http://www.parzival.unibe.ch/hsverz.html#70"]</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -3060,7 +3060,7 @@
         <v>130</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D95">
         <v>47.994247999999999</v>
@@ -3070,7 +3070,7 @@
       </c>
       <c r="F95" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 54 (Gψ)","https://heinztschan.github.io/parzival/show_library.html?lat=47.994248&amp;lng=7.845004&amp;lib=Freiburg i. Br.&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#71"]</v>
+        <v xml:space="preserve">  -  ["Fr. 54 (Gψ)","https://heinztschan.github.io/parzival/show_library.html?lat=47.994248&amp;lng=7.845004&amp;lib=Freiburg i. Br.&amp;url=http://www.parzival.unibe.ch/hsverz.html#71"]</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -3081,7 +3081,7 @@
         <v>3</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D96">
         <v>48.205874999999999</v>
@@ -3091,7 +3091,7 @@
       </c>
       <c r="F96" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 55 (B)","https://heinztschan.github.io/parzival/show_library.html?lat=48.205875&amp;lng=16.366904&amp;lib=Wien&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#72"]</v>
+        <v xml:space="preserve">  -  ["Fr. 55 (B)","https://heinztschan.github.io/parzival/show_library.html?lat=48.205875&amp;lng=16.366904&amp;lib=Wien&amp;url=http://www.parzival.unibe.ch/hsverz.html#72"]</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -3102,7 +3102,7 @@
         <v>128</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D97">
         <v>48.297263999999998</v>
@@ -3112,7 +3112,7 @@
       </c>
       <c r="F97" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 56 (C )","https://heinztschan.github.io/parzival/show_library.html?lat=48.297264&amp;lng=14.290971&amp;lib=Linz&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#73"]</v>
+        <v xml:space="preserve">  -  ["Fr. 56 (C )","https://heinztschan.github.io/parzival/show_library.html?lat=48.297264&amp;lng=14.290971&amp;lib=Linz&amp;url=http://www.parzival.unibe.ch/hsverz.html#73"]</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -3123,7 +3123,7 @@
         <v>7</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D98">
         <v>49.403415000000003</v>
@@ -3133,7 +3133,7 @@
       </c>
       <c r="F98" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 57 (H)","https://heinztschan.github.io/parzival/show_library.html?lat=49.403415&amp;lng=8.675165&amp;lib=Heidelberg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#74"]</v>
+        <v xml:space="preserve">  -  ["Fr. 57 (H)","https://heinztschan.github.io/parzival/show_library.html?lat=49.403415&amp;lng=8.675165&amp;lib=Heidelberg&amp;url=http://www.parzival.unibe.ch/hsverz.html#74"]</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -3144,7 +3144,7 @@
         <v>130</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D99">
         <v>47.994247999999999</v>
@@ -3154,7 +3154,7 @@
       </c>
       <c r="F99" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 58 (q)","https://heinztschan.github.io/parzival/show_library.html?lat=47.994248&amp;lng=7.845004&amp;lib=Freiburg i. Br.&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#75"]</v>
+        <v xml:space="preserve">  -  ["Fr. 58 (q)","https://heinztschan.github.io/parzival/show_library.html?lat=47.994248&amp;lng=7.845004&amp;lib=Freiburg i. Br.&amp;url=http://www.parzival.unibe.ch/hsverz.html#75"]</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -3165,7 +3165,7 @@
         <v>134</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D100">
         <v>50.803550000000001</v>
@@ -3175,7 +3175,7 @@
       </c>
       <c r="F100" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 59","https://heinztschan.github.io/parzival/show_library.html?lat=50.80355&amp;lng=8.76291&amp;lib=Marburg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#76"]</v>
+        <v xml:space="preserve">  -  ["Fr. 59","https://heinztschan.github.io/parzival/show_library.html?lat=50.80355&amp;lng=8.76291&amp;lib=Marburg&amp;url=http://www.parzival.unibe.ch/hsverz.html#76"]</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -3186,7 +3186,7 @@
         <v>136</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D101">
         <v>46.047519999999999</v>
@@ -3196,7 +3196,7 @@
       </c>
       <c r="F101" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 60","https://heinztschan.github.io/parzival/show_library.html?lat=46.04752&amp;lng=14.503967&amp;lib=Ljubljana&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#77"]</v>
+        <v xml:space="preserve">  -  ["Fr. 60","https://heinztschan.github.io/parzival/show_library.html?lat=46.04752&amp;lng=14.503967&amp;lib=Ljubljana&amp;url=http://www.parzival.unibe.ch/hsverz.html#77"]</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -3207,7 +3207,7 @@
         <v>7</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D102">
         <v>49.403415000000003</v>
@@ -3217,7 +3217,7 @@
       </c>
       <c r="F102" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 61","https://heinztschan.github.io/parzival/show_library.html?lat=49.403415&amp;lng=8.675165&amp;lib=Heidelberg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#78"]</v>
+        <v xml:space="preserve">  -  ["Fr. 61","https://heinztschan.github.io/parzival/show_library.html?lat=49.403415&amp;lng=8.675165&amp;lib=Heidelberg&amp;url=http://www.parzival.unibe.ch/hsverz.html#78"]</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -3228,7 +3228,7 @@
         <v>139</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D103">
         <v>53.203479999999999</v>
@@ -3238,7 +3238,7 @@
       </c>
       <c r="F103" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 62","https://heinztschan.github.io/parzival/show_library.html?lat=53.20348&amp;lng=5.790048&amp;lib=Leeuwarden&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#79"]</v>
+        <v xml:space="preserve">  -  ["Fr. 62","https://heinztschan.github.io/parzival/show_library.html?lat=53.20348&amp;lng=5.790048&amp;lib=Leeuwarden&amp;url=http://www.parzival.unibe.ch/hsverz.html#79"]</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -3249,7 +3249,7 @@
         <v>3</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D104">
         <v>48.213185000000003</v>
@@ -3259,7 +3259,7 @@
       </c>
       <c r="F104" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 63","https://heinztschan.github.io/parzival/show_library.html?lat=48.213185&amp;lng=16.36005&amp;lib=Wien&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#80"]</v>
+        <v xml:space="preserve">  -  ["Fr. 63","https://heinztschan.github.io/parzival/show_library.html?lat=48.213185&amp;lng=16.36005&amp;lib=Wien&amp;url=http://www.parzival.unibe.ch/hsverz.html#80"]</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -3270,7 +3270,7 @@
         <v>142</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D105">
         <v>51.366239</v>
@@ -3280,7 +3280,7 @@
       </c>
       <c r="F105" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 64","https://heinztschan.github.io/parzival/show_library.html?lat=51.366239&amp;lng=8.989292&amp;lib=Mengeringhausen&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#81"]</v>
+        <v xml:space="preserve">  -  ["Fr. 64","https://heinztschan.github.io/parzival/show_library.html?lat=51.366239&amp;lng=8.989292&amp;lib=Mengeringhausen&amp;url=http://www.parzival.unibe.ch/hsverz.html#81"]</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -3291,7 +3291,7 @@
         <v>144</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D106">
         <v>52.369503999999999</v>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="F106" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 65","https://heinztschan.github.io/parzival/show_library.html?lat=52.369504&amp;lng=9.730706&amp;lib=Hannover&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#82"]</v>
+        <v xml:space="preserve">  -  ["Fr. 65","https://heinztschan.github.io/parzival/show_library.html?lat=52.369504&amp;lng=9.730706&amp;lib=Hannover&amp;url=http://www.parzival.unibe.ch/hsverz.html#82"]</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -3312,7 +3312,7 @@
         <v>146</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D107">
         <v>48.334539999999997</v>
@@ -3322,7 +3322,7 @@
       </c>
       <c r="F107" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 66","https://heinztschan.github.io/parzival/show_library.html?lat=48.33454&amp;lng=10.895091&amp;lib=Augsburg&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#83"]</v>
+        <v xml:space="preserve">  -  ["Fr. 66","https://heinztschan.github.io/parzival/show_library.html?lat=48.33454&amp;lng=10.895091&amp;lib=Augsburg&amp;url=http://www.parzival.unibe.ch/hsverz.html#83"]</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -3333,7 +3333,7 @@
         <v>64</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D108">
         <v>48.797629999999998</v>
@@ -3343,7 +3343,7 @@
       </c>
       <c r="F108" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 67","https://heinztschan.github.io/parzival/show_library.html?lat=48.79763&amp;lng=9.2251&amp;lib=Stuttgart&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#84"]</v>
+        <v xml:space="preserve">  -  ["Fr. 67","https://heinztschan.github.io/parzival/show_library.html?lat=48.79763&amp;lng=9.2251&amp;lib=Stuttgart&amp;url=http://www.parzival.unibe.ch/hsverz.html#84"]</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -3354,7 +3354,7 @@
         <v>149</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D109">
         <v>51.844647000000002</v>
@@ -3364,7 +3364,7 @@
       </c>
       <c r="F109" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 68","https://heinztschan.github.io/parzival/show_library.html?lat=51.844647&amp;lng=6.427598&amp;lib=Schloss Anholt&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#85"]</v>
+        <v xml:space="preserve">  -  ["Fr. 68","https://heinztschan.github.io/parzival/show_library.html?lat=51.844647&amp;lng=6.427598&amp;lib=Schloss Anholt&amp;url=http://www.parzival.unibe.ch/hsverz.html#85"]</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -3375,7 +3375,7 @@
         <v>150</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D110">
         <v>50.937531</v>
@@ -3385,7 +3385,7 @@
       </c>
       <c r="F110" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 68","https://heinztschan.github.io/parzival/show_library.html?lat=50.937531&amp;lng=6.960279&amp;lib=Köln&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#85"]</v>
+        <v xml:space="preserve">  -  ["Fr. 68","https://heinztschan.github.io/parzival/show_library.html?lat=50.937531&amp;lng=6.960279&amp;lib=Köln&amp;url=http://www.parzival.unibe.ch/hsverz.html#85"]</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -3396,7 +3396,7 @@
         <v>88</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D111">
         <v>47.208827999999997</v>
@@ -3406,7 +3406,7 @@
       </c>
       <c r="F111" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 69","https://heinztschan.github.io/parzival/show_library.html?lat=47.208828&amp;lng=7.532055&amp;lib=Solothurn&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#86"]</v>
+        <v xml:space="preserve">  -  ["Fr. 69","https://heinztschan.github.io/parzival/show_library.html?lat=47.208828&amp;lng=7.532055&amp;lib=Solothurn&amp;url=http://www.parzival.unibe.ch/hsverz.html#86"]</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -3417,7 +3417,7 @@
         <v>153</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D112">
         <v>51.980564000000001</v>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="F112" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 70","https://heinztschan.github.io/parzival/show_library.html?lat=51.980564&amp;lng=5.904767&amp;lib=Arnhem&amp;url=http://http://www.parzival.unibe.ch/hsverz.html87"]</v>
+        <v xml:space="preserve">  -  ["Fr. 70","https://heinztschan.github.io/parzival/show_library.html?lat=51.980564&amp;lng=5.904767&amp;lib=Arnhem&amp;url=http://www.parzival.unibe.ch/hsverz.html87"]</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -3438,7 +3438,7 @@
         <v>125</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D113">
         <v>50.079951000000001</v>
@@ -3448,7 +3448,7 @@
       </c>
       <c r="F113" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  -  ["Fr. 71","https://heinztschan.github.io/parzival/show_library.html?lat=50.079951&amp;lng=14.431825&amp;lib=Praha&amp;url=http://http://www.parzival.unibe.ch/hsverz.html#88"]</v>
+        <v xml:space="preserve">  -  ["Fr. 71","https://heinztschan.github.io/parzival/show_library.html?lat=50.079951&amp;lng=14.431825&amp;lib=Praha&amp;url=http://www.parzival.unibe.ch/hsverz.html#88"]</v>
       </c>
     </row>
   </sheetData>
@@ -3500,64 +3500,64 @@
     <hyperlink ref="C47" r:id="rId45" location="40" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
     <hyperlink ref="C48" r:id="rId46" location="40" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
     <hyperlink ref="C49" r:id="rId47" location="41" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="C53" r:id="rId48" location="42" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="C54" r:id="rId49" location="43" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="C55" r:id="rId50" location="44" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="C56" r:id="rId51" location="45" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="C57" r:id="rId52" location="45" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="C58" r:id="rId53" location="46" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="C59" r:id="rId54" location="47" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="C60" r:id="rId55" location="48" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="C61" r:id="rId56" location="48" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="C62" r:id="rId57" location="49" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="C63" r:id="rId58" location="49" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="C64" r:id="rId59" location="50" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="C65" r:id="rId60" location="51" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="C66" r:id="rId61" location="52" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="C67" r:id="rId62" location="53" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="C68" r:id="rId63" location="54" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="C69" r:id="rId64" location="55" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="C70" r:id="rId65" location="56" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="C71" r:id="rId66" location="56" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="C72" r:id="rId67" location="57" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="C76" r:id="rId68" location="58" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="C77" r:id="rId69" location="59" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="C78" r:id="rId70" location="60" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="C79" r:id="rId71" location="61" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="C80" r:id="rId72" location="62" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="C81" r:id="rId73" location="62" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="C82" r:id="rId74" location="63" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="C83" r:id="rId75" location="64" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="C84" r:id="rId76" location="64" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="C85" r:id="rId77" location="65" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="C86" r:id="rId78" location="65" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="C87" r:id="rId79" location="65" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="C88" r:id="rId80" location="66" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="C89" r:id="rId81" location="67" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="C90" r:id="rId82" location="67" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="C91" r:id="rId83" location="68" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="C92" r:id="rId84" location="68" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="C93" r:id="rId85" location="69" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="C94" r:id="rId86" location="70" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="C95" r:id="rId87" location="71" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="C96" r:id="rId88" location="72" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="C97" r:id="rId89" location="73" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="C98" r:id="rId90" location="74" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="C99" r:id="rId91" location="75" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="C100" r:id="rId92" location="76" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="C101" r:id="rId93" location="77" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="C102" r:id="rId94" location="78" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="C103" r:id="rId95" location="79" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="C104" r:id="rId96" location="80" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="C105" r:id="rId97" location="81" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="C106" r:id="rId98" location="82" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="C107" r:id="rId99" location="83" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="C108" r:id="rId100" location="84" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="C109" r:id="rId101" location="85" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="C110" r:id="rId102" location="85" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="C111" r:id="rId103" location="86" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="C112" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="C113" r:id="rId105" location="88" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="C53" r:id="rId48" location="42" display="http://www.parzival.unibe.ch/hsverz.html#42" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="C54" r:id="rId49" location="43" display="http://www.parzival.unibe.ch/hsverz.html#43" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="C55" r:id="rId50" location="44" display="http://www.parzival.unibe.ch/hsverz.html#44" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="C56" r:id="rId51" location="45" display="http://www.parzival.unibe.ch/hsverz.html#45" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="C57" r:id="rId52" location="45" display="http://www.parzival.unibe.ch/hsverz.html#45" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="C58" r:id="rId53" location="46" display="http://www.parzival.unibe.ch/hsverz.html#46" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="C59" r:id="rId54" location="47" display="http://www.parzival.unibe.ch/hsverz.html#47" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="C60" r:id="rId55" location="48" display="http://www.parzival.unibe.ch/hsverz.html#48" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="C61" r:id="rId56" location="48" display="http://www.parzival.unibe.ch/hsverz.html#48" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="C62" r:id="rId57" location="49" display="http://www.parzival.unibe.ch/hsverz.html#49" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="C63" r:id="rId58" location="49" display="http://www.parzival.unibe.ch/hsverz.html#49" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="C64" r:id="rId59" location="50" display="http://www.parzival.unibe.ch/hsverz.html#50" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="C65" r:id="rId60" location="51" display="http://www.parzival.unibe.ch/hsverz.html#51" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="C66" r:id="rId61" location="52" display="http://www.parzival.unibe.ch/hsverz.html#52" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="C67" r:id="rId62" location="53" display="http://www.parzival.unibe.ch/hsverz.html#53" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="C68" r:id="rId63" location="54" display="http://www.parzival.unibe.ch/hsverz.html#54" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="C69" r:id="rId64" location="55" display="http://www.parzival.unibe.ch/hsverz.html#55" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="C70" r:id="rId65" location="56" display="http://www.parzival.unibe.ch/hsverz.html#56" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="C71" r:id="rId66" location="56" display="http://www.parzival.unibe.ch/hsverz.html#56" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="C72" r:id="rId67" location="57" display="http://www.parzival.unibe.ch/hsverz.html#57" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="C76" r:id="rId68" location="58" display="http://www.parzival.unibe.ch/hsverz.html#58" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="C77" r:id="rId69" location="59" display="http://www.parzival.unibe.ch/hsverz.html#59" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="C78" r:id="rId70" location="60" display="http://www.parzival.unibe.ch/hsverz.html#60" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="C79" r:id="rId71" location="61" display="http://www.parzival.unibe.ch/hsverz.html#61" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="C80" r:id="rId72" location="62" display="http://www.parzival.unibe.ch/hsverz.html#62" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="C81" r:id="rId73" location="62" display="http://www.parzival.unibe.ch/hsverz.html#62" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="C82" r:id="rId74" location="63" display="http://www.parzival.unibe.ch/hsverz.html#63" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="C83" r:id="rId75" location="64" display="http://www.parzival.unibe.ch/hsverz.html#64" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="C84" r:id="rId76" location="64" display="http://www.parzival.unibe.ch/hsverz.html#64" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="C85" r:id="rId77" location="65" display="http://www.parzival.unibe.ch/hsverz.html#65" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="C86" r:id="rId78" location="65" display="http://www.parzival.unibe.ch/hsverz.html#65" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="C87" r:id="rId79" location="65" display="http://www.parzival.unibe.ch/hsverz.html#65" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="C88" r:id="rId80" location="66" display="http://www.parzival.unibe.ch/hsverz.html#66" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="C89" r:id="rId81" location="67" display="http://www.parzival.unibe.ch/hsverz.html#67" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="C90" r:id="rId82" location="67" display="http://www.parzival.unibe.ch/hsverz.html#67" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="C91" r:id="rId83" location="68" display="http://www.parzival.unibe.ch/hsverz.html#68" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="C92" r:id="rId84" location="68" display="http://www.parzival.unibe.ch/hsverz.html#68" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="C93" r:id="rId85" location="69" display="http://www.parzival.unibe.ch/hsverz.html#69" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="C94" r:id="rId86" location="70" display="http://www.parzival.unibe.ch/hsverz.html#70" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="C95" r:id="rId87" location="71" display="http://www.parzival.unibe.ch/hsverz.html#71" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="C96" r:id="rId88" location="72" display="http://www.parzival.unibe.ch/hsverz.html#72" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="C97" r:id="rId89" location="73" display="http://www.parzival.unibe.ch/hsverz.html#73" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="C98" r:id="rId90" location="74" display="http://www.parzival.unibe.ch/hsverz.html#74" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="C99" r:id="rId91" location="75" display="http://www.parzival.unibe.ch/hsverz.html#75" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="C100" r:id="rId92" location="76" display="http://www.parzival.unibe.ch/hsverz.html#76" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="C101" r:id="rId93" location="77" display="http://www.parzival.unibe.ch/hsverz.html#77" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="C102" r:id="rId94" location="78" display="http://www.parzival.unibe.ch/hsverz.html#78" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="C103" r:id="rId95" location="79" display="http://www.parzival.unibe.ch/hsverz.html#79" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="C104" r:id="rId96" location="80" display="http://www.parzival.unibe.ch/hsverz.html#80" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="C105" r:id="rId97" location="81" display="http://www.parzival.unibe.ch/hsverz.html#81" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="C106" r:id="rId98" location="82" display="http://www.parzival.unibe.ch/hsverz.html#82" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="C107" r:id="rId99" location="83" display="http://www.parzival.unibe.ch/hsverz.html#83" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="C108" r:id="rId100" location="84" display="http://www.parzival.unibe.ch/hsverz.html#84" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="C109" r:id="rId101" location="85" display="http://www.parzival.unibe.ch/hsverz.html#85" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="C110" r:id="rId102" location="85" display="http://www.parzival.unibe.ch/hsverz.html#85" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="C111" r:id="rId103" location="86" display="http://www.parzival.unibe.ch/hsverz.html#86" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="C112" r:id="rId104" display="http://www.parzival.unibe.ch/hsverz.html87" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="C113" r:id="rId105" location="88" display="http://www.parzival.unibe.ch/hsverz.html#88" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId106"/>

</xml_diff>